<commit_message>
Add the ability to verify file size and file type logic.
</commit_message>
<xml_diff>
--- a/src/main/resources/Web_Data.xlsx
+++ b/src/main/resources/Web_Data.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\code\0011_LeviBI\LeviBI-backendnew\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Code\LeviBI\LeviBI-backend\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC11A10D-CB1C-4E9B-8CFD-4850D55CB763}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5025" yWindow="5025" windowWidth="28800" windowHeight="15345" xr2:uid="{229EEA6E-F8A7-2545-904A-8F0032855BE1}"/>
+    <workbookView xWindow="5030" yWindow="5030" windowWidth="28800" windowHeight="15350"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,14 +34,47 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>日期</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>用户数</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2号</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>3号</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>4号</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>5号</t>
+  </si>
+  <si>
+    <t>6号</t>
+  </si>
+  <si>
+    <t>7号</t>
+  </si>
+  <si>
+    <t>8号</t>
+  </si>
+  <si>
+    <t>9号</t>
+  </si>
+  <si>
+    <t>10号</t>
+  </si>
+  <si>
+    <t>11号</t>
   </si>
   <si>
     <r>
@@ -50,65 +82,45 @@
     </r>
     <r>
       <rPr>
-        <sz val="10"/>
+        <sz val="11"/>
         <rFont val="宋体"/>
         <family val="2"/>
         <charset val="134"/>
       </rPr>
       <t>号</t>
     </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2号</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>3号</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>4号</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>5号</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="176" formatCode="yyyy/m/d\ h:mm;@"/>
+    <numFmt numFmtId="164" formatCode="yyyy/m/d\ h:mm;@"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
       <sz val="18"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="宋体"/>
-      <family val="2"/>
-      <charset val="134"/>
     </font>
     <font>
       <sz val="16"/>
@@ -117,12 +129,10 @@
       <charset val="134"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="等线"/>
+      <sz val="11"/>
+      <name val="宋体"/>
       <family val="2"/>
       <charset val="134"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -162,18 +172,17 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -487,94 +496,379 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{260829AF-83D5-9D43-A57C-13A2BDCFFDE0}">
-  <dimension ref="A1:D12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.07421875" defaultRowHeight="23.25" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11.0546875" defaultRowHeight="23.5"/>
   <cols>
-    <col min="4" max="4" width="10.765625" style="1"/>
+    <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.77734375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:14">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D1"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:14">
+      <c r="A2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="2">
+        <v>10</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+    </row>
+    <row r="3" spans="1:14">
+      <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B3" s="2">
+        <v>20</v>
+      </c>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+    </row>
+    <row r="4" spans="1:14">
+      <c r="A4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2">
+        <v>30</v>
+      </c>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+    </row>
+    <row r="5" spans="1:14">
+      <c r="A5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2">
+        <v>40</v>
+      </c>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+    </row>
+    <row r="6" spans="1:14">
+      <c r="A6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2">
+        <v>50</v>
+      </c>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+    </row>
+    <row r="7" spans="1:14">
+      <c r="A7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2">
+        <v>9</v>
+      </c>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
+    </row>
+    <row r="8" spans="1:14">
+      <c r="A8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="2">
+        <v>6</v>
+      </c>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
+    </row>
+    <row r="9" spans="1:14">
+      <c r="A9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="2">
+        <v>1</v>
+      </c>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
+      <c r="N9" s="2"/>
+    </row>
+    <row r="10" spans="1:14">
+      <c r="A10" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="2">
+        <v>22</v>
+      </c>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
+      <c r="L10" s="2"/>
+      <c r="M10" s="2"/>
+      <c r="N10" s="2"/>
+    </row>
+    <row r="11" spans="1:14">
+      <c r="A11" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D2"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="4">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A4" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="4">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="3">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="3">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B7" s="1"/>
-      <c r="D7"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B8" s="1"/>
-      <c r="D8"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B9" s="1"/>
-      <c r="D9"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B10" s="1"/>
-      <c r="D10"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B11" s="1"/>
-      <c r="D11"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B12" s="1"/>
-      <c r="D12"/>
+      <c r="B11" s="2">
+        <v>11</v>
+      </c>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
+      <c r="L11" s="2"/>
+      <c r="M11" s="2"/>
+      <c r="N11" s="2"/>
+    </row>
+    <row r="12" spans="1:14">
+      <c r="A12" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="2">
+        <v>21</v>
+      </c>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
+      <c r="L12" s="2"/>
+      <c r="M12" s="2"/>
+      <c r="N12" s="2"/>
+    </row>
+    <row r="13" spans="1:14">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="2"/>
+      <c r="L13" s="2"/>
+      <c r="M13" s="2"/>
+      <c r="N13" s="2"/>
+    </row>
+    <row r="14" spans="1:14">
+      <c r="A14" s="2"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
+      <c r="L14" s="2"/>
+      <c r="M14" s="2"/>
+      <c r="N14" s="2"/>
+    </row>
+    <row r="15" spans="1:14">
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2"/>
+      <c r="K15" s="2"/>
+      <c r="L15" s="2"/>
+      <c r="M15" s="2"/>
+      <c r="N15" s="2"/>
+    </row>
+    <row r="16" spans="1:14">
+      <c r="A16" s="2"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
+      <c r="K16" s="2"/>
+      <c r="L16" s="2"/>
+      <c r="M16" s="2"/>
+      <c r="N16" s="2"/>
+    </row>
+    <row r="17" spans="1:14">
+      <c r="A17" s="2"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+      <c r="I17" s="2"/>
+      <c r="J17" s="2"/>
+      <c r="K17" s="2"/>
+      <c r="L17" s="2"/>
+      <c r="M17" s="2"/>
+      <c r="N17" s="2"/>
+    </row>
+    <row r="18" spans="1:14">
+      <c r="A18" s="2"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
+      <c r="J18" s="2"/>
+      <c r="K18" s="2"/>
+      <c r="L18" s="2"/>
+      <c r="M18" s="2"/>
+      <c r="N18" s="2"/>
+    </row>
+    <row r="19" spans="1:14">
+      <c r="A19" s="2"/>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
+      <c r="I19" s="2"/>
+      <c r="J19" s="2"/>
+      <c r="K19" s="2"/>
+      <c r="L19" s="2"/>
+      <c r="M19" s="2"/>
+      <c r="N19" s="2"/>
+    </row>
+    <row r="20" spans="1:14">
+      <c r="A20" s="2"/>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
+      <c r="H20" s="2"/>
+      <c r="I20" s="2"/>
+      <c r="J20" s="2"/>
+      <c r="K20" s="2"/>
+      <c r="L20" s="2"/>
+      <c r="M20" s="2"/>
+      <c r="N20" s="2"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>